<commit_message>
Dagbaekur Ivan Gusti Saevar uddfaerdar
</commit_message>
<xml_diff>
--- a/Dagbaekur/Sævar/DagbokS.xlsx
+++ b/Dagbaekur/Sævar/DagbokS.xlsx
@@ -1,17 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="105" windowWidth="20730" windowHeight="11055"/>
+    <workbookView xWindow="-15" yWindow="6390" windowWidth="28830" windowHeight="6435"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
@@ -96,8 +96,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -251,6 +251,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -285,6 +286,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -460,19 +462,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:J62"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+      <selection activeCell="J60" sqref="J60"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="12.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:10">
+    <row r="2" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B2" s="4" t="s">
         <v>0</v>
       </c>
@@ -486,7 +488,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="4" spans="2:10">
+    <row r="4" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>15</v>
       </c>
@@ -512,7 +514,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="2:10">
+    <row r="5" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C5" s="1">
         <v>41659</v>
       </c>
@@ -535,7 +537,7 @@
         <v>41665</v>
       </c>
     </row>
-    <row r="6" spans="2:10">
+    <row r="6" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>3</v>
       </c>
@@ -547,7 +549,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="7" spans="2:10">
+    <row r="7" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>1</v>
       </c>
@@ -556,7 +558,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="2:10">
+    <row r="8" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>2</v>
       </c>
@@ -565,7 +567,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="2:10">
+    <row r="9" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>4</v>
       </c>
@@ -574,7 +576,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="2:10">
+    <row r="10" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>5</v>
       </c>
@@ -583,7 +585,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="2:10">
+    <row r="11" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B11" s="2" t="s">
         <v>6</v>
       </c>
@@ -599,7 +601,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="2:10">
+    <row r="12" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B12" s="3" t="s">
         <v>14</v>
       </c>
@@ -608,7 +610,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="14" spans="2:10">
+    <row r="14" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
         <v>16</v>
       </c>
@@ -634,7 +636,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="2:10">
+    <row r="15" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C15" s="1">
         <v>41301</v>
       </c>
@@ -657,7 +659,7 @@
         <v>41307</v>
       </c>
     </row>
-    <row r="16" spans="2:10">
+    <row r="16" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>3</v>
       </c>
@@ -669,7 +671,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="17" spans="2:10">
+    <row r="17" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
         <v>1</v>
       </c>
@@ -684,7 +686,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="18" spans="2:10">
+    <row r="18" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
         <v>2</v>
       </c>
@@ -696,19 +698,19 @@
         <v>180</v>
       </c>
     </row>
-    <row r="19" spans="2:10">
+    <row r="19" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
         <v>4</v>
       </c>
       <c r="H19">
-        <v>60</v>
+        <v>120</v>
       </c>
       <c r="J19">
         <f t="shared" si="1"/>
-        <v>60</v>
-      </c>
-    </row>
-    <row r="20" spans="2:10">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="20" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
         <v>5</v>
       </c>
@@ -717,7 +719,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="2:10">
+    <row r="21" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B21" s="2" t="s">
         <v>6</v>
       </c>
@@ -733,16 +735,16 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="2:10">
+    <row r="22" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B22" s="3" t="s">
         <v>14</v>
       </c>
       <c r="J22">
         <f>SUM(J16:J21)</f>
-        <v>480</v>
-      </c>
-    </row>
-    <row r="24" spans="2:10">
+        <v>540</v>
+      </c>
+    </row>
+    <row r="24" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
         <v>18</v>
       </c>
@@ -768,7 +770,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="25" spans="2:10">
+    <row r="25" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C25" s="1">
         <v>41673</v>
       </c>
@@ -791,7 +793,7 @@
         <v>41679</v>
       </c>
     </row>
-    <row r="26" spans="2:10">
+    <row r="26" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
         <v>3</v>
       </c>
@@ -800,7 +802,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="2:10">
+    <row r="27" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
         <v>1</v>
       </c>
@@ -809,7 +811,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="2:10">
+    <row r="28" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
         <v>2</v>
       </c>
@@ -824,7 +826,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="29" spans="2:10">
+    <row r="29" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
         <v>4</v>
       </c>
@@ -842,7 +844,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="30" spans="2:10">
+    <row r="30" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
         <v>5</v>
       </c>
@@ -851,7 +853,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="2:10">
+    <row r="31" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B31" s="2" t="s">
         <v>6</v>
       </c>
@@ -867,7 +869,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="2:10">
+    <row r="32" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B32" s="3" t="s">
         <v>14</v>
       </c>
@@ -876,7 +878,7 @@
         <v>720</v>
       </c>
     </row>
-    <row r="34" spans="2:10">
+    <row r="34" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
         <v>19</v>
       </c>
@@ -902,7 +904,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="35" spans="2:10">
+    <row r="35" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C35" s="1">
         <v>41680</v>
       </c>
@@ -925,16 +927,22 @@
         <v>41686</v>
       </c>
     </row>
-    <row r="36" spans="2:10">
+    <row r="36" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
         <v>3</v>
       </c>
+      <c r="C36">
+        <v>0</v>
+      </c>
+      <c r="D36">
+        <v>60</v>
+      </c>
       <c r="J36">
         <f>SUM(C36:I36)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="37" spans="2:10">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="37" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B37" t="s">
         <v>1</v>
       </c>
@@ -943,34 +951,52 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="2:10">
+    <row r="38" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B38" t="s">
         <v>2</v>
       </c>
+      <c r="D38">
+        <v>60</v>
+      </c>
+      <c r="E38">
+        <v>60</v>
+      </c>
       <c r="J38">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="39" spans="2:10">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="39" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B39" t="s">
         <v>4</v>
       </c>
+      <c r="C39">
+        <v>180</v>
+      </c>
+      <c r="D39">
+        <v>360</v>
+      </c>
+      <c r="E39">
+        <v>240</v>
+      </c>
       <c r="J39">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="40" spans="2:10">
+        <v>780</v>
+      </c>
+    </row>
+    <row r="40" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B40" t="s">
         <v>5</v>
       </c>
+      <c r="E40">
+        <v>60</v>
+      </c>
       <c r="J40">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="41" spans="2:10">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="41" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B41" s="2" t="s">
         <v>6</v>
       </c>
@@ -986,16 +1012,16 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="2:10">
+    <row r="42" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B42" s="3" t="s">
         <v>14</v>
       </c>
       <c r="J42">
         <f>SUM(J36:J41)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="44" spans="2:10">
+        <v>1020</v>
+      </c>
+    </row>
+    <row r="44" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B44" t="s">
         <v>22</v>
       </c>
@@ -1021,7 +1047,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="45" spans="2:10">
+    <row r="45" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C45" s="1">
         <v>41687</v>
       </c>
@@ -1044,7 +1070,7 @@
         <v>41693</v>
       </c>
     </row>
-    <row r="46" spans="2:10">
+    <row r="46" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B46" t="s">
         <v>3</v>
       </c>
@@ -1053,7 +1079,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="2:10">
+    <row r="47" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B47" t="s">
         <v>1</v>
       </c>
@@ -1062,7 +1088,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="2:10">
+    <row r="48" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B48" t="s">
         <v>2</v>
       </c>
@@ -1071,64 +1097,80 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="2:10">
+    <row r="49" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B49" t="s">
         <v>4</v>
       </c>
+      <c r="C49">
+        <v>150</v>
+      </c>
+      <c r="D49">
+        <v>240</v>
+      </c>
+      <c r="E49">
+        <v>180</v>
+      </c>
       <c r="J49">
         <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="50" spans="2:10">
+        <v>570</v>
+      </c>
+    </row>
+    <row r="50" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B50" t="s">
         <v>5</v>
       </c>
+      <c r="D50">
+        <v>60</v>
+      </c>
       <c r="J50">
         <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="51" spans="2:10">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="51" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B51" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C51" s="2"/>
-      <c r="D51" s="2"/>
-      <c r="E51" s="2"/>
+      <c r="D51" s="2">
+        <v>60</v>
+      </c>
+      <c r="E51" s="2">
+        <v>120</v>
+      </c>
       <c r="F51" s="2"/>
       <c r="G51" s="2"/>
       <c r="H51" s="2"/>
       <c r="I51" s="2"/>
       <c r="J51" s="2">
         <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="52" spans="2:10">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="52" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B52" s="3" t="s">
         <v>14</v>
       </c>
       <c r="J52">
         <f>SUM(J46:J51)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="54" spans="2:10">
+        <v>810</v>
+      </c>
+    </row>
+    <row r="54" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B54" s="4" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="56" spans="2:10">
+    <row r="56" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B56" t="s">
         <v>3</v>
       </c>
       <c r="D56">
         <f t="shared" ref="D56:D61" si="5">J6+J16+J26+J36</f>
-        <v>150</v>
-      </c>
-    </row>
-    <row r="57" spans="2:10">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="57" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B57" t="s">
         <v>1</v>
       </c>
@@ -1137,34 +1179,34 @@
         <v>180</v>
       </c>
     </row>
-    <row r="58" spans="2:10">
+    <row r="58" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B58" t="s">
         <v>2</v>
       </c>
       <c r="D58">
         <f t="shared" si="5"/>
-        <v>300</v>
-      </c>
-    </row>
-    <row r="59" spans="2:10">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="59" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B59" t="s">
         <v>4</v>
       </c>
       <c r="D59">
         <f t="shared" si="5"/>
-        <v>660</v>
-      </c>
-    </row>
-    <row r="60" spans="2:10">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="60" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B60" t="s">
         <v>5</v>
       </c>
       <c r="D60">
         <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="61" spans="2:10">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="61" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B61" s="2" t="s">
         <v>6</v>
       </c>
@@ -1174,13 +1216,17 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="2:10">
+    <row r="62" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B62" s="3" t="s">
         <v>21</v>
       </c>
       <c r="D62" s="3">
-        <f>SUM(D56:D61)</f>
-        <v>1290</v>
+        <f>SUM(J12,J22,J32,J42,J52)</f>
+        <v>3180</v>
+      </c>
+      <c r="F62">
+        <f>D62/60</f>
+        <v>53</v>
       </c>
     </row>
   </sheetData>
@@ -1193,24 +1239,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>